<commit_message>
Logging Fabio Puissant 10-12-2020
</commit_message>
<xml_diff>
--- a/Logging_Fabio.xlsx
+++ b/Logging_Fabio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiopuissant/UHasselt/Software Engineering/inf-seng-20-21-team-projectgroep-10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045D0861-D860-4F49-95FA-557DD11D2019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6EA4AF-9F0B-494F-B4EA-CD9D272DD161}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task List Fabio" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="54">
   <si>
     <t>TASK</t>
   </si>
@@ -179,6 +179,30 @@
   </si>
   <si>
     <t>Brainstormen  de nieuwe &gt; scope, rollen, taken en use cases noteren voor de uitgebreide scope veeteelt</t>
+  </si>
+  <si>
+    <t>Meeting implementern feedback probleemomschrijving</t>
+  </si>
+  <si>
+    <t>Probleemomschrijving uitgebreidt beschrijven, zorgen dat iedereeen hetzelfde idee heeft over de functies uit de nieuwe, verbeterde projectomschrijving.</t>
+  </si>
+  <si>
+    <t>Uitschrijven van het subdeel 'rollen en rechten' voor de probleemstelling.</t>
+  </si>
+  <si>
+    <t>Probleemomschrijving uitbreiden</t>
+  </si>
+  <si>
+    <t>Meeting Analyse Sprint</t>
+  </si>
+  <si>
+    <t>Bespreken wat er tijdens de analyse moet gebreuren; Taakverdeling; Aanpak;</t>
+  </si>
+  <si>
+    <t>Functionele requirements opstellen</t>
+  </si>
+  <si>
+    <t>Eerste 36 functionele voorlopige requirements uitgeschreven.</t>
   </si>
 </sst>
 </file>
@@ -436,7 +460,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -514,13 +544,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -702,15 +726,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ToDoList" displayName="ToDoList" ref="B2:H17" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ToDoList" displayName="ToDoList" ref="B2:H21" totalsRowShown="0">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TASK"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PRIORITY "/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="STATUS "/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="START DATE " dataCellStyle="Date"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="DUE DATE " dataCellStyle="Date"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="HOURS WORKED" dataDxfId="1" dataCellStyle="Per cent"/>
-    <tableColumn id="5" xr3:uid="{78C56347-6357-9244-81CF-2384BCAA30AF}" name="NOTES" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="HOURS WORKED" dataDxfId="10" dataCellStyle="Per cent"/>
+    <tableColumn id="5" xr3:uid="{78C56347-6357-9244-81CF-2384BCAA30AF}" name="NOTES" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="To-do list" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -729,8 +753,8 @@
     <tableColumn id="4" xr3:uid="{08343B73-5922-1F4A-B1B6-8BD0E5A41E25}" name="STATUS "/>
     <tableColumn id="6" xr3:uid="{1A6ABB63-28E7-8143-8DEF-16BFFBACEE09}" name="START DATE " dataCellStyle="Date"/>
     <tableColumn id="7" xr3:uid="{10AB3798-2BB1-744B-87CE-102A9EDC3ACB}" name="DUE DATE " dataCellStyle="Date"/>
-    <tableColumn id="10" xr3:uid="{82B04305-6997-C845-806A-AB5C2672DF04}" name="HOURS WORKED" dataDxfId="9" dataCellStyle="Per cent"/>
-    <tableColumn id="5" xr3:uid="{78A7A19A-F09B-9643-8B8A-3B3CF7BB1A45}" name="NOTES" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{82B04305-6997-C845-806A-AB5C2672DF04}" name="HOURS WORKED" dataDxfId="7" dataCellStyle="Per cent"/>
+    <tableColumn id="5" xr3:uid="{78A7A19A-F09B-9643-8B8A-3B3CF7BB1A45}" name="NOTES" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="To-do list" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -749,8 +773,8 @@
     <tableColumn id="4" xr3:uid="{6C3DB45E-15AD-6D45-B2F7-1586E2EBA779}" name="STATUS "/>
     <tableColumn id="6" xr3:uid="{BF9C8E9D-6589-0143-95EF-3AF3DFA62B85}" name="START DATE " dataCellStyle="Date"/>
     <tableColumn id="7" xr3:uid="{A724884B-7097-8146-B989-9D02FD4864CE}" name="DUE DATE " dataCellStyle="Date"/>
-    <tableColumn id="10" xr3:uid="{1D6CB921-DFAC-F14B-BA58-3FD08A59A7B2}" name="HOURS WORKED" dataDxfId="6" dataCellStyle="Per cent"/>
-    <tableColumn id="5" xr3:uid="{6B743C2B-2BD0-8641-AD58-FC1961A87F42}" name="NOTES" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{1D6CB921-DFAC-F14B-BA58-3FD08A59A7B2}" name="HOURS WORKED" dataDxfId="4" dataCellStyle="Per cent"/>
+    <tableColumn id="5" xr3:uid="{6B743C2B-2BD0-8641-AD58-FC1961A87F42}" name="NOTES" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="To-do list" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -769,8 +793,8 @@
     <tableColumn id="4" xr3:uid="{56B4C51E-0B8E-304C-89EC-F36DDC7218F6}" name="STATUS "/>
     <tableColumn id="6" xr3:uid="{49E9A012-34F6-134D-83DD-762339356686}" name="START DATE " dataCellStyle="Date"/>
     <tableColumn id="7" xr3:uid="{BF7252B0-8FCB-B64F-B151-CF8CACBD611D}" name="DUE DATE " dataCellStyle="Date"/>
-    <tableColumn id="10" xr3:uid="{574B9FFA-9DA2-ED49-9908-BC58972B4866}" name="HOURS WORKED" dataDxfId="3" dataCellStyle="Per cent"/>
-    <tableColumn id="5" xr3:uid="{83077B79-F877-2D48-BCD9-AEFC907B0744}" name="NOTES" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{574B9FFA-9DA2-ED49-9908-BC58972B4866}" name="HOURS WORKED" dataDxfId="1" dataCellStyle="Per cent"/>
+    <tableColumn id="5" xr3:uid="{83077B79-F877-2D48-BCD9-AEFC907B0744}" name="NOTES" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="To-do list" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -1012,10 +1036,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I17"/>
+  <dimension ref="B1:I21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1"/>
@@ -1024,8 +1048,8 @@
     <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="16.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="49" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" customWidth="1"/>
+    <col min="8" max="8" width="63.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
     <col min="10" max="10" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1093,7 +1117,7 @@
       </c>
       <c r="I3" s="9">
         <f>SUM(ToDoList[HOURS WORKED])</f>
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1">
@@ -1395,7 +1419,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="3:8" ht="30" customHeight="1">
+    <row r="17" spans="2:8" ht="30" customHeight="1">
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>5</v>
       </c>
@@ -1403,20 +1430,109 @@
         <v>11</v>
       </c>
       <c r="E17" s="2">
+        <v>44168</v>
+      </c>
+      <c r="F17" s="2">
+        <v>44168</v>
+      </c>
+      <c r="G17" s="14">
+        <v>2</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="30" customHeight="1">
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2">
+        <v>44168</v>
+      </c>
+      <c r="F18" s="2">
+        <v>44168</v>
+      </c>
+      <c r="G18" s="14">
+        <v>1</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="30" customHeight="1">
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2">
+        <v>44175</v>
+      </c>
+      <c r="F19" s="2">
+        <v>44175</v>
+      </c>
+      <c r="G19" s="14">
+        <v>2</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="30" customHeight="1">
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="2">
+        <v>44175</v>
+      </c>
+      <c r="F20" s="2">
+        <v>44184</v>
+      </c>
+      <c r="G20" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="30" customHeight="1">
+      <c r="C21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="2">
+        <v>44131</v>
+      </c>
+      <c r="F21" s="2">
         <v>44139</v>
       </c>
-      <c r="F17" s="2">
-        <v>44139</v>
-      </c>
-      <c r="G17" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="H17" s="15"/>
+      <c r="G21" s="14">
+        <v>0</v>
+      </c>
+      <c r="H21" s="15"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B13:F13 C14:F17">
+  <conditionalFormatting sqref="B13:F13 C14:F21">
     <cfRule type="expression" dxfId="11" priority="14">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
@@ -1429,13 +1545,13 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Status in this column under this heading.  Press ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="D2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in this column under this heading" sqref="E2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Due Date in this column under this heading" sqref="F2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="C13:C17" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="C13:C21" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>"Low, Normal, High"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="D13:D17" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="D13:D21" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"Not Started, In Progress, Deferred, Complete"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="hours worked on task" prompt="Enter a Nummeric value (Decimal or Whole) for the hours worked on this task " sqref="G13:G17" xr:uid="{2CAE7E5B-2E18-F847-86E5-AC7789E67A7B}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="hours worked on task" prompt="Enter a Nummeric value (Decimal or Whole) for the hours worked on this task " sqref="G2:G21" xr:uid="{57FA1E33-ABF3-9D4A-BF05-395E4DACFE16}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -1525,11 +1641,11 @@
       </c>
       <c r="E3" s="2">
         <f ca="1">TODAY()</f>
-        <v>44145</v>
+        <v>44175</v>
       </c>
       <c r="F3" s="2">
         <f ca="1">ToDoList2[[#This Row],[START DATE ]]+7</f>
-        <v>44152</v>
+        <v>44182</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1551,11 +1667,11 @@
       </c>
       <c r="E4" s="2">
         <f ca="1">TODAY()-30</f>
-        <v>44115</v>
+        <v>44145</v>
       </c>
       <c r="F4" s="2">
         <f ca="1">ToDoList2[[#This Row],[START DATE ]]+35</f>
-        <v>44150</v>
+        <v>44180</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -1573,11 +1689,11 @@
       </c>
       <c r="E5" s="2">
         <f ca="1">TODAY()-23</f>
-        <v>44122</v>
+        <v>44152</v>
       </c>
       <c r="F5" s="2">
         <f ca="1">ToDoList2[[#This Row],[START DATE ]]+10</f>
-        <v>44132</v>
+        <v>44162</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -1642,21 +1758,21 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="B3:F13">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="hours worked on task" prompt="Enter a Nummeric value (Decimal or Whole) for the hours worked on this task " sqref="G3:G17" xr:uid="{FA4850AA-191D-C54C-8088-A0C5510AF946}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="hours worked on task" prompt="Enter a Nummeric value (Decimal or Whole) for the hours worked on this task " sqref="G3:G21" xr:uid="{FA4850AA-191D-C54C-8088-A0C5510AF946}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The Due Date must be greater than or equal to the Start Date. Select YES to keep the value, NO to retry or CANCEL to clear the entry" sqref="F3:F17" xr:uid="{364325AB-25DE-EC46-8A5E-AE3D9349460A}">
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The Due Date must be greater than or equal to the Start Date. Select YES to keep the value, NO to retry or CANCEL to clear the entry" sqref="F3:F21" xr:uid="{364325AB-25DE-EC46-8A5E-AE3D9349460A}">
       <formula1>F3&gt;=E3</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="D3:D17" xr:uid="{79B56497-027B-8E4B-9E60-01AACC729BC4}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="D3:D21" xr:uid="{79B56497-027B-8E4B-9E60-01AACC729BC4}">
       <formula1>"Not Started, In Progress, Deferred, Complete"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="C3:C17" xr:uid="{C5919058-A463-8A49-8BB8-6623BCC20CA7}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="C3:C21" xr:uid="{C5919058-A463-8A49-8BB8-6623BCC20CA7}">
       <formula1>"Low, Normal, High"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Due Date in this column under this heading" sqref="F2" xr:uid="{38366972-6BAD-ED49-820F-15C57DA24E8D}"/>
@@ -1753,11 +1869,11 @@
       </c>
       <c r="E3" s="2">
         <f ca="1">TODAY()</f>
-        <v>44145</v>
+        <v>44175</v>
       </c>
       <c r="F3" s="2">
         <f ca="1">ToDoList3[[#This Row],[START DATE ]]+7</f>
-        <v>44152</v>
+        <v>44182</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1779,11 +1895,11 @@
       </c>
       <c r="E4" s="2">
         <f ca="1">TODAY()-30</f>
-        <v>44115</v>
+        <v>44145</v>
       </c>
       <c r="F4" s="2">
         <f ca="1">ToDoList3[[#This Row],[START DATE ]]+35</f>
-        <v>44150</v>
+        <v>44180</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -1801,11 +1917,11 @@
       </c>
       <c r="E5" s="2">
         <f ca="1">TODAY()-23</f>
-        <v>44122</v>
+        <v>44152</v>
       </c>
       <c r="F5" s="2">
         <f ca="1">ToDoList3[[#This Row],[START DATE ]]+10</f>
-        <v>44132</v>
+        <v>44162</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -1870,21 +1986,21 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="B3:F13">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="hours worked on task" prompt="Enter a Nummeric value (Decimal or Whole) for the hours worked on this task " sqref="G3:G17" xr:uid="{356A63AD-56A3-DA4A-98E2-5AF307F31BDB}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="hours worked on task" prompt="Enter a Nummeric value (Decimal or Whole) for the hours worked on this task " sqref="G3:G21" xr:uid="{356A63AD-56A3-DA4A-98E2-5AF307F31BDB}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The Due Date must be greater than or equal to the Start Date. Select YES to keep the value, NO to retry or CANCEL to clear the entry" sqref="F3:F17" xr:uid="{E85DA8D5-068A-7B49-B9E7-434F71539885}">
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The Due Date must be greater than or equal to the Start Date. Select YES to keep the value, NO to retry or CANCEL to clear the entry" sqref="F3:F21" xr:uid="{E85DA8D5-068A-7B49-B9E7-434F71539885}">
       <formula1>F3&gt;=E3</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="D3:D17" xr:uid="{875A503B-259B-B142-AD55-B17724B0976D}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="D3:D21" xr:uid="{875A503B-259B-B142-AD55-B17724B0976D}">
       <formula1>"Not Started, In Progress, Deferred, Complete"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="C3:C17" xr:uid="{C7165301-3BB0-4944-8AF3-CD678355808F}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="C3:C21" xr:uid="{C7165301-3BB0-4944-8AF3-CD678355808F}">
       <formula1>"Low, Normal, High"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Due Date in this column under this heading" sqref="F2" xr:uid="{77D48218-7B93-0340-82A3-A578717FF107}"/>
@@ -1981,11 +2097,11 @@
       </c>
       <c r="E3" s="2">
         <f ca="1">TODAY()</f>
-        <v>44145</v>
+        <v>44175</v>
       </c>
       <c r="F3" s="2">
         <f ca="1">ToDoList34[[#This Row],[START DATE ]]+7</f>
-        <v>44152</v>
+        <v>44182</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2007,11 +2123,11 @@
       </c>
       <c r="E4" s="2">
         <f ca="1">TODAY()-30</f>
-        <v>44115</v>
+        <v>44145</v>
       </c>
       <c r="F4" s="2">
         <f ca="1">ToDoList34[[#This Row],[START DATE ]]+35</f>
-        <v>44150</v>
+        <v>44180</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -2029,11 +2145,11 @@
       </c>
       <c r="E5" s="2">
         <f ca="1">TODAY()-23</f>
-        <v>44122</v>
+        <v>44152</v>
       </c>
       <c r="F5" s="2">
         <f ca="1">ToDoList34[[#This Row],[START DATE ]]+10</f>
-        <v>44132</v>
+        <v>44162</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -2098,7 +2214,7 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="B3:F13">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2110,16 +2226,16 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Status in this column under this heading.  Press ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="D2" xr:uid="{275103DB-4B36-354F-A152-921FEA99272A}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in this column under this heading" sqref="E2" xr:uid="{B0C57800-60CE-364D-B862-8A8D72DC6AAC}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Due Date in this column under this heading" sqref="F2" xr:uid="{863D0563-08BD-244A-A90F-97D0D984A9BC}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="C3:C17" xr:uid="{FFCA7491-2AEA-EE47-8145-1D46BFA04D3E}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="C3:C21" xr:uid="{FFCA7491-2AEA-EE47-8145-1D46BFA04D3E}">
       <formula1>"Low, Normal, High"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="D3:D17" xr:uid="{DFC06829-7713-0340-AC90-3651D32D2CE8}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="D3:D21" xr:uid="{DFC06829-7713-0340-AC90-3651D32D2CE8}">
       <formula1>"Not Started, In Progress, Deferred, Complete"</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The Due Date must be greater than or equal to the Start Date. Select YES to keep the value, NO to retry or CANCEL to clear the entry" sqref="F3:F17" xr:uid="{7CC77FE1-F0D6-FC40-8FC7-AC0B41FB6CD4}">
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The Due Date must be greater than or equal to the Start Date. Select YES to keep the value, NO to retry or CANCEL to clear the entry" sqref="F3:F21" xr:uid="{7CC77FE1-F0D6-FC40-8FC7-AC0B41FB6CD4}">
       <formula1>F3&gt;=E3</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="hours worked on task" prompt="Enter a Nummeric value (Decimal or Whole) for the hours worked on this task " sqref="G3:G17" xr:uid="{8532DE81-4E7A-D74B-9BCD-9342D44CE07D}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="hours worked on task" prompt="Enter a Nummeric value (Decimal or Whole) for the hours worked on this task " sqref="G3:G21" xr:uid="{8532DE81-4E7A-D74B-9BCD-9342D44CE07D}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>